<commit_message>
[WIP] Intentando ajustar el clasificador para distinga entre productos, soporte u otros por el momento no funciona correctamente.
</commit_message>
<xml_diff>
--- a/productos.xlsx
+++ b/productos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\crmia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB7EF0D-8E86-493C-9AAE-2D06F39CFB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7A83AB-6887-40D8-BE63-FD2AEB7EF803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5250" windowWidth="29040" windowHeight="15720" xr2:uid="{E318524F-57B9-411D-B6CE-7269314643C4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>ID</t>
   </si>
@@ -84,6 +84,12 @@
   </si>
   <si>
     <t>Televisor UHD Smart TV.</t>
+  </si>
+  <si>
+    <t>Lavadora 15kg</t>
+  </si>
+  <si>
+    <t>Lavadora automática de 15 kg.</t>
   </si>
 </sst>
 </file>
@@ -476,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E0BD62-906A-449D-A462-F4815941CEAE}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,6 +587,23 @@
       </c>
       <c r="F5" s="1"/>
     </row>
+    <row r="6" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2">
+        <v>10000</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>